<commit_message>
up to date till 10-3-20
</commit_message>
<xml_diff>
--- a/BloodstreamAPI/testData/session.xlsx
+++ b/BloodstreamAPI/testData/session.xlsx
@@ -3,15 +3,16 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B309B38-7082-4866-A517-BBDF1F3CE019}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{6583602A-4089-41BE-B0CB-81B1E305C536}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14685" windowHeight="5745" tabRatio="715" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13740" windowHeight="9585" tabRatio="715" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="logoff" sheetId="2" r:id="rId1"/>
     <sheet name="heartbeat" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
+  <oleSize ref="A1:N29"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="5">
   <si>
     <t>EndPoint</t>
   </si>
@@ -35,7 +36,7 @@
     <t>/session/loginToken</t>
   </si>
   <si>
-    <t>Assert404</t>
+    <t>/session/heartbeat</t>
   </si>
 </sst>
 </file>
@@ -402,7 +403,7 @@
   <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD12"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -450,9 +451,7 @@
       <c r="E4" s="2"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
-        <v>4</v>
-      </c>
+      <c r="A5" s="6"/>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
       <c r="D5" s="6"/>
@@ -463,18 +462,14 @@
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
-      <c r="E6" s="3" t="s">
-        <v>0</v>
-      </c>
+      <c r="E6" s="3"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
-      <c r="E7" s="5" t="s">
-        <v>3</v>
-      </c>
+      <c r="E7" s="5"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
@@ -529,7 +524,7 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="A5" sqref="A5:E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -558,7 +553,7 @@
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
       <c r="E3" s="5" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -569,9 +564,7 @@
       <c r="E4" s="2"/>
     </row>
     <row r="5" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
-        <v>4</v>
-      </c>
+      <c r="A5" s="6"/>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
       <c r="D5" s="6"/>
@@ -582,18 +575,14 @@
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
-      <c r="E6" s="3" t="s">
-        <v>0</v>
-      </c>
+      <c r="E6" s="3"/>
     </row>
     <row r="7" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
-      <c r="E7" s="5" t="s">
-        <v>3</v>
-      </c>
+      <c r="E7" s="5"/>
     </row>
     <row r="8" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
@@ -626,7 +615,7 @@
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
       <c r="E11" s="5" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -637,5 +626,6 @@
     <mergeCell ref="A9:E9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>